<commit_message>
Dashboard shows current data and time. Erased test records in database
</commit_message>
<xml_diff>
--- a/IEEE_Shop.xlsx
+++ b/IEEE_Shop.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="inventory 24-01-2024" sheetId="1" r:id="rId1"/>
-    <sheet name="bought_items 24-01-2024" sheetId="2" r:id="rId2"/>
+    <sheet name="inventory 28-01-2024" sheetId="1" r:id="rId1"/>
+    <sheet name="transactions 28-01-2024" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>barcode</t>
   </si>
@@ -38,79 +38,22 @@
     <t>last_check_in</t>
   </si>
   <si>
-    <t>111111111111</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>1234566</t>
-  </si>
-  <si>
-    <t>12345666</t>
-  </si>
-  <si>
-    <t>123456667</t>
-  </si>
-  <si>
-    <t>AHHHHHHH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ooh Ahh </t>
-  </si>
-  <si>
-    <t>CHECK THE TIME</t>
-  </si>
-  <si>
-    <t>Test Show 2</t>
-  </si>
-  <si>
-    <t>Test Show 3</t>
-  </si>
-  <si>
-    <t>Test Show 4</t>
-  </si>
-  <si>
-    <t>Geez</t>
-  </si>
-  <si>
-    <t>Snack</t>
-  </si>
-  <si>
-    <t>Meh</t>
-  </si>
-  <si>
-    <t>ACHOO</t>
+    <t>112233</t>
+  </si>
+  <si>
+    <t>Doritos</t>
+  </si>
+  <si>
+    <t>Snacks</t>
   </si>
   <si>
     <t>Walmart</t>
   </si>
   <si>
-    <t>Sum Tin Mart</t>
-  </si>
-  <si>
-    <t>15-01-2024 10:54:06</t>
-  </si>
-  <si>
-    <t>19-01-2024 12:54:04</t>
-  </si>
-  <si>
-    <t>20-01-2024 16:50:25</t>
-  </si>
-  <si>
-    <t>19-01-2024 12:56:01</t>
-  </si>
-  <si>
-    <t>19-01-2024 12:56:11</t>
-  </si>
-  <si>
-    <t>19-01-2024 12:56:21</t>
-  </si>
-  <si>
-    <t>23-01-2024 14:41:48</t>
+    <t>25-01-2024 16:27:28</t>
+  </si>
+  <si>
+    <t>25-01-2024 16:49:56</t>
   </si>
 </sst>
 </file>
@@ -468,13 +411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="B1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="2:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,162 +438,6 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>9.25</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>2.05</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>2.05</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>2.05</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +447,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -694,25 +481,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>2.5</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -720,25 +507,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>2.5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>2.05</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -746,25 +533,77 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2.5</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>2.05</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug where 0 is first number at checkout
</commit_message>
<xml_diff>
--- a/IEEE_Shop.xlsx
+++ b/IEEE_Shop.xlsx
@@ -7,15 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="inventory 28-01-2024" sheetId="1" r:id="rId1"/>
-    <sheet name="transactions 28-01-2024" sheetId="2" r:id="rId2"/>
+    <sheet name="inventory 30-01-2024" sheetId="1" r:id="rId1"/>
+    <sheet name="transactions 30-01-2024" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
   <si>
     <t>barcode</t>
   </si>
@@ -38,15 +38,66 @@
     <t>last_check_in</t>
   </si>
   <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>045496870775</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>Cheetos</t>
+  </si>
+  <si>
+    <t>Doritos</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
+    <t>mwe</t>
+  </si>
+  <si>
+    <t>Costco</t>
+  </si>
+  <si>
+    <t>zerg</t>
+  </si>
+  <si>
+    <t>30-01-2024 14:15:31</t>
+  </si>
+  <si>
+    <t>30-01-2024 14:13:23</t>
+  </si>
+  <si>
+    <t>30-01-2024 14:16:22</t>
+  </si>
+  <si>
+    <t>30-01-2024 14:28:21</t>
+  </si>
+  <si>
+    <t>30-01-2024 14:28:32</t>
+  </si>
+  <si>
     <t>112233</t>
   </si>
   <si>
-    <t>Doritos</t>
-  </si>
-  <si>
-    <t>Snacks</t>
-  </si>
-  <si>
     <t>Walmart</t>
   </si>
   <si>
@@ -54,6 +105,9 @@
   </si>
   <si>
     <t>25-01-2024 16:49:56</t>
+  </si>
+  <si>
+    <t>30-01-2024 14:29:18</t>
   </si>
 </sst>
 </file>
@@ -411,13 +465,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,6 +492,136 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>2.5</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>3.45</v>
+      </c>
+      <c r="E4">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>2.5</v>
+      </c>
+      <c r="E5">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>3.5</v>
+      </c>
+      <c r="E6">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -447,7 +631,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -481,10 +665,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>2.5</v>
@@ -493,13 +677,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -507,10 +691,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>2.5</v>
@@ -519,13 +703,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -533,10 +717,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>2.5</v>
@@ -545,13 +729,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -559,10 +743,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>2.5</v>
@@ -571,13 +755,13 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -585,10 +769,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>2.5</v>
@@ -597,13 +781,91 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="G6" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>3.45</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
-        <v>12</v>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>2.5</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>3.5</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>